<commit_message>
Update Elektrobox_Stückliste/ Add Schalplan
</commit_message>
<xml_diff>
--- a/Stuecklisten/Elektrobox_Stückliste.xlsx
+++ b/Stuecklisten/Elektrobox_Stückliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HTL\SPL\CandyMaschine_Project\CandyMachine_Watermelon\Stuecklisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619B425C-BB8C-4E60-95B2-7FA3DB295B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDACB8BC-2BF2-49A1-81AC-C6530BDDBCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9960" xr2:uid="{9DA56051-2903-42FB-B064-034924F5A5D2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{9DA56051-2903-42FB-B064-034924F5A5D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>Artikelnummer</t>
   </si>
   <si>
-    <t>Arduino Mega</t>
-  </si>
-  <si>
     <t>Spannungsverteiler</t>
   </si>
   <si>
@@ -68,18 +65,12 @@
     <t>Taster</t>
   </si>
   <si>
-    <t>https://store.arduino.cc/products/arduino-mega-2560-rev3?queryID=undefined</t>
-  </si>
-  <si>
     <t>https://www.amazon.de/TB6612FNG-Dual-DC-Schrittmotor-Treibermodul-Dual-Treiber-Controller-Platine-H-Brücke-DC-Schritt/dp/B09MN8F1SD/ref=sr_1_1_sspa?adgrpid=69037961897&amp;dib=eyJ2IjoiMSJ9.6_jIzgScYGB7l6JCbOjHO5S3JMlqMJTovkJvTOiZ6Vnn7io60PzXR5Vm7BvLbgtAul56yl4dwjh6Z5Wtb-pxvnJb49nq6BDzk671MJVkhjsoKU_FwBjNFw9UEOxQZX6nWXy286mOuE7LNsbDcLUWeb2xe9g-TP0oBOoKSSjN_S2KuvZzBiu3xEI5iQnjUiHiqY9MQL5Uxo6mJm0yQ1EUV3onOxW2JPE-nEnH4OafhlVcqIeLV_wKHfqFCqQa4_9pFScr2FRymo2R6wU95qG7zO_YmeTyMkqkprA14e00rbg.-3TRibSq9BgltuAFmCibi6UvqsT9uL_1Nj_0woe9aDE&amp;dib_tag=se&amp;hvadid=596128743118&amp;hvdev=c&amp;hvexpln=0&amp;hvlocphy=9197120&amp;hvnetw=g&amp;hvocijid=7099133041148048338--&amp;hvqmt=e&amp;hvrand=7099133041148048338&amp;hvtargid=kwd-298108739501&amp;hydadcr=29220_2368110&amp;keywords=tb6612fng&amp;mcid=b76250beeb7238568bad9ee8746f39fc&amp;qid=1766130313&amp;sr=8-1-spons&amp;aref=tapiZomnNp&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;psc=1</t>
   </si>
   <si>
     <t>‎Hyuduoaticw0mh6k3131</t>
   </si>
   <si>
-    <t>A000067</t>
-  </si>
-  <si>
     <t>Verdrahtungskanal</t>
   </si>
   <si>
@@ -102,6 +93,15 @@
   </si>
   <si>
     <t>0,99€/Stück</t>
+  </si>
+  <si>
+    <t>Arduino Uno</t>
+  </si>
+  <si>
+    <t>https://store-usa.arduino.cc/products/arduino-uno-rev3?queryID=a151cf05c686d58ddc787acc986795cd</t>
+  </si>
+  <si>
+    <t>A000066</t>
   </si>
 </sst>
 </file>
@@ -149,12 +149,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -175,6 +169,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0F1111"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -220,20 +220,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -670,7 +670,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,16 +703,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="5">
-        <v>52.8</v>
+        <v>20</v>
+      </c>
+      <c r="C2" s="4">
+        <v>20.7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -720,15 +720,15 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="7">
+        <v>14</v>
+      </c>
+      <c r="C3" s="6">
         <v>5.87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="10">
+        <v>5</v>
+      </c>
+      <c r="E3" s="9">
         <v>108785</v>
       </c>
     </row>
@@ -737,16 +737,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="7">
+        <v>15</v>
+      </c>
+      <c r="C4" s="6">
         <v>8.0500000000000007</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -754,16 +754,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="7">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6">
         <v>24.19</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -771,16 +771,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="6">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5">
         <v>9.8800000000000008</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -788,15 +788,15 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="11">
+        <v>8</v>
+      </c>
+      <c r="E7" s="10">
         <v>2050005748030</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Elektrobox_Stückliste/ Add 2. Version of Schaltplan
</commit_message>
<xml_diff>
--- a/Stuecklisten/Elektrobox_Stückliste.xlsx
+++ b/Stuecklisten/Elektrobox_Stückliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HTL\SPL\CandyMaschine_Project\CandyMachine_Watermelon\Stuecklisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDACB8BC-2BF2-49A1-81AC-C6530BDDBCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76A4B39-49B1-4D43-A47D-08B486A93626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{9DA56051-2903-42FB-B064-034924F5A5D2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Anzahl</t>
   </si>
@@ -65,12 +65,6 @@
     <t>Taster</t>
   </si>
   <si>
-    <t>https://www.amazon.de/TB6612FNG-Dual-DC-Schrittmotor-Treibermodul-Dual-Treiber-Controller-Platine-H-Brücke-DC-Schritt/dp/B09MN8F1SD/ref=sr_1_1_sspa?adgrpid=69037961897&amp;dib=eyJ2IjoiMSJ9.6_jIzgScYGB7l6JCbOjHO5S3JMlqMJTovkJvTOiZ6Vnn7io60PzXR5Vm7BvLbgtAul56yl4dwjh6Z5Wtb-pxvnJb49nq6BDzk671MJVkhjsoKU_FwBjNFw9UEOxQZX6nWXy286mOuE7LNsbDcLUWeb2xe9g-TP0oBOoKSSjN_S2KuvZzBiu3xEI5iQnjUiHiqY9MQL5Uxo6mJm0yQ1EUV3onOxW2JPE-nEnH4OafhlVcqIeLV_wKHfqFCqQa4_9pFScr2FRymo2R6wU95qG7zO_YmeTyMkqkprA14e00rbg.-3TRibSq9BgltuAFmCibi6UvqsT9uL_1Nj_0woe9aDE&amp;dib_tag=se&amp;hvadid=596128743118&amp;hvdev=c&amp;hvexpln=0&amp;hvlocphy=9197120&amp;hvnetw=g&amp;hvocijid=7099133041148048338--&amp;hvqmt=e&amp;hvrand=7099133041148048338&amp;hvtargid=kwd-298108739501&amp;hydadcr=29220_2368110&amp;keywords=tb6612fng&amp;mcid=b76250beeb7238568bad9ee8746f39fc&amp;qid=1766130313&amp;sr=8-1-spons&amp;aref=tapiZomnNp&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;psc=1</t>
-  </si>
-  <si>
-    <t>‎Hyuduoaticw0mh6k3131</t>
-  </si>
-  <si>
     <t>Verdrahtungskanal</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>B0DG8Z24NN</t>
   </si>
   <si>
-    <t>https://www.automation24.at/verteilerblock-phoenix-1300611-ptvfix-2-5-5?previewPriceListId=1&amp;refID=adwords_shopping_AT&amp;gad_source=1&amp;gad_campaignid=20923317010&amp;gclid=CjwKCAiAvaLLBhBFEiwAYCNTf44v4z6j4oBw7kaow1k46yQAHDHvTJey5UjswNzXvyg3IMF55D5GdhoCQzwQAvD_BwE</t>
-  </si>
-  <si>
     <t>https://www.amazon.de/Spannungs-wandler-Aideepen-Spannungs-regler-Convertermit-Kabelschnittstelle/dp/B0CLRSFL13/ref=sr_1_6?dib=eyJ2IjoiMSJ9.iNDu1-G-hZSMpfKt3KWQqsizmOTcYsYdeO2m0vULZM_UYmGP2L0Uu20hEGeYqkcLr4cjI8LYJIXPR8kVq0czpqGZIl0VCpBIpxlGvgm-q4w_TyiOcCevbTvSzmemBj0379m8slUqp9kocFUlyzWhWErd8Ur4JCNzqblAo8_Xk6NSWKrziujtADu9lubJ_Oud6ZNk17QPVhdYKVY_XBjkGo2EGX_CN0wL8Mc7AvgPTvyDyksc9hjqLexgsVDCZBo3T3LF3aNnpds4ziIuFFaA5ZlESrvCntYASwP1AIsQCak.R0lnyivqmDQa180s2ByuqBlWvAulUb9ms-w3STDRGtk&amp;dib_tag=se&amp;keywords=spannungswandler%2B12v%2B5v&amp;qid=1768547011&amp;sr=8-6&amp;th=1</t>
   </si>
   <si>
@@ -102,6 +93,18 @@
   </si>
   <si>
     <t>A000066</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/AZDelivery-Controller-AZ-L298N-Logische-Spannung/dp/B0BV79NX3B?th=1</t>
+  </si>
+  <si>
+    <t>B0BV79NX3B</t>
+  </si>
+  <si>
+    <t>https://at.rs-online.com/web/p/idc-steckverbinder/6257252</t>
+  </si>
+  <si>
+    <t>304-04-769</t>
   </si>
 </sst>
 </file>
@@ -156,12 +159,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF555555"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -175,6 +172,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF393939"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -225,14 +228,12 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -670,7 +671,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,16 +704,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4">
         <v>20.7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -720,16 +721,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C3" s="6">
-        <v>5.87</v>
+        <v>5.26</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="9">
-        <v>108785</v>
+      <c r="E3" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -737,7 +738,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" s="6">
         <v>8.0500000000000007</v>
@@ -746,7 +747,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -754,16 +755,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="6">
         <v>24.19</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -771,16 +772,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5">
-        <v>9.8800000000000008</v>
+        <v>8.56</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -788,26 +789,25 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>2050005748030</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{4A34E0FF-3A6E-4F69-A963-1E8C7B7DF937}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://www.automation24.at/verteilerblock-phoenix-1300611-ptvfix-2-5-5?previewPriceListId=1&amp;refID=adwords_shopping_AT&amp;gad_source=1&amp;gad_campaignid=20923317010&amp;gclid=CjwKCAiAvaLLBhBFEiwAYCNTf44v4z6j4oBw7kaow1k46yQAHDHvTJey5UjswNzXvyg3IMF55D5GdhoCQzwQAvD_BwE" xr:uid="{8A95B3DD-5AFC-44E8-806A-C621FB829850}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://www.amazon.de/Spannungs-wandler-Aideepen-Spannungs-regler-Convertermit-Kabelschnittstelle/dp/B0CLRSFL13/ref=sr_1_6?dib=eyJ2IjoiMSJ9.iNDu1-G-hZSMpfKt3KWQqsizmOTcYsYdeO2m0vULZM_UYmGP2L0Uu20hEGeYqkcLr4cjI8LYJIXPR8kVq0czpqGZIl0VCpBIpxlGvgm-q4w_TyiOcCevbTvSzmemBj0379m8slUqp9kocFUlyzWhWErd8Ur4JCNzqblAo8_Xk6NSWKrziujtADu9lubJ_Oud6ZNk17QPVhdYKVY_XBjkGo2EGX_CN0wL8Mc7AvgPTvyDyksc9hjqLexgsVDCZBo3T3LF3aNnpds4ziIuFFaA5ZlESrvCntYASwP1AIsQCak.R0lnyivqmDQa180s2ByuqBlWvAulUb9ms-w3STDRGtk&amp;dib_tag=se&amp;keywords=spannungswandler%2B12v%2B5v&amp;qid=1768547011&amp;sr=8-6&amp;th=1" xr:uid="{23BD11BB-0F37-4191-8468-10AC86A9F4FE}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.amazon.de/Spannungs-wandler-Aideepen-Spannungs-regler-Convertermit-Kabelschnittstelle/dp/B0CLRSFL13/ref=sr_1_6?dib=eyJ2IjoiMSJ9.iNDu1-G-hZSMpfKt3KWQqsizmOTcYsYdeO2m0vULZM_UYmGP2L0Uu20hEGeYqkcLr4cjI8LYJIXPR8kVq0czpqGZIl0VCpBIpxlGvgm-q4w_TyiOcCevbTvSzmemBj0379m8slUqp9kocFUlyzWhWErd8Ur4JCNzqblAo8_Xk6NSWKrziujtADu9lubJ_Oud6ZNk17QPVhdYKVY_XBjkGo2EGX_CN0wL8Mc7AvgPTvyDyksc9hjqLexgsVDCZBo3T3LF3aNnpds4ziIuFFaA5ZlESrvCntYASwP1AIsQCak.R0lnyivqmDQa180s2ByuqBlWvAulUb9ms-w3STDRGtk&amp;dib_tag=se&amp;keywords=spannungswandler%2B12v%2B5v&amp;qid=1768547011&amp;sr=8-6&amp;th=1" xr:uid="{23BD11BB-0F37-4191-8468-10AC86A9F4FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Stückliste Elektrobox Rahmen
</commit_message>
<xml_diff>
--- a/Stuecklisten/Elektrobox_Stückliste.xlsx
+++ b/Stuecklisten/Elektrobox_Stückliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HTL\SPL\CandyMaschine_Project\CandyMachine_Watermelon\Stuecklisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9C53D0-C05F-40ED-9CB0-9269509ECD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB4C4F6-D5ED-4562-8343-F1392741895F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{9DA56051-2903-42FB-B064-034924F5A5D2}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9960" xr2:uid="{9DA56051-2903-42FB-B064-034924F5A5D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -92,16 +92,16 @@
     <t>B0BV79NX3B</t>
   </si>
   <si>
-    <t>https://at.rs-online.com/web/p/idc-steckverbinder/6257252</t>
-  </si>
-  <si>
-    <t>304-04-769</t>
-  </si>
-  <si>
     <t>https://www.reichelt.com/de/en/shop/product/arduino_nano_esp32_with_header_esp32-s3_usb-c-353087?country=de&amp;CCTYPE=private&amp;LANGUAGE=en</t>
   </si>
   <si>
     <t>Arduino Nano</t>
+  </si>
+  <si>
+    <t>https://at.rs-online.com/web/p/idc-steckverbinder/0471187</t>
+  </si>
+  <si>
+    <t>471-187</t>
   </si>
 </sst>
 </file>
@@ -188,7 +188,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -203,6 +203,15 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBEBEBE"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -231,9 +240,11 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -671,7 +682,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,15 +715,15 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4">
         <v>19.8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="11">
+        <v>19</v>
+      </c>
+      <c r="E2" s="10">
         <v>7630049203969</v>
       </c>
     </row>
@@ -721,16 +732,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="6">
-        <v>5.26</v>
+        <v>5.29</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>19</v>
+      <c r="E3" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -771,7 +782,7 @@
       <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="5">
@@ -788,7 +799,7 @@
       <c r="A7" s="2">
         <v>2</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -804,9 +815,13 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="https://www.amazon.de/Spannungs-wandler-Aideepen-Spannungs-regler-Convertermit-Kabelschnittstelle/dp/B0CLRSFL13/ref=sr_1_6?dib=eyJ2IjoiMSJ9.iNDu1-G-hZSMpfKt3KWQqsizmOTcYsYdeO2m0vULZM_UYmGP2L0Uu20hEGeYqkcLr4cjI8LYJIXPR8kVq0czpqGZIl0VCpBIpxlGvgm-q4w_TyiOcCevbTvSzmemBj0379m8slUqp9kocFUlyzWhWErd8Ur4JCNzqblAo8_Xk6NSWKrziujtADu9lubJ_Oud6ZNk17QPVhdYKVY_XBjkGo2EGX_CN0wL8Mc7AvgPTvyDyksc9hjqLexgsVDCZBo3T3LF3aNnpds4ziIuFFaA5ZlESrvCntYASwP1AIsQCak.R0lnyivqmDQa180s2ByuqBlWvAulUb9ms-w3STDRGtk&amp;dib_tag=se&amp;keywords=spannungswandler%2B12v%2B5v&amp;qid=1768547011&amp;sr=8-6&amp;th=1" xr:uid="{23BD11BB-0F37-4191-8468-10AC86A9F4FE}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00BC4F0C-D697-4CE4-8278-4A347B796AA4}"/>
+    <hyperlink ref="B7" r:id="rId3" display="https://www.conrad.at/de/p/tru-components-yst-1102a-drucktaster-12-v-dc-0-05-a-1-x-aus-ein-tastend-l-x-b-6-mm-x-6-mm-1-st-1569018.html?insert=UP&amp;utm_source=google-shopping-de&amp;utm_medium=search&amp;utm_campaign=shopping-online-de&amp;utm_content=shopping-ad_cpc&amp;WT.srch=1&amp;ef_id=CjwKCAiAvaLLBhBFEiwAYCNTf908VSnv0s-MmemZj0iv06QLJpiNhpOEHccYiJTgeAskNOWtXxIFdhoCrUYQAvD_BwE:G:s&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_AT_2025&amp;utm_id=22317741252&amp;gad_source=1&amp;gad_campaignid=22317741252&amp;gclid=CjwKCAiAvaLLBhBFEiwAYCNTf908VSnv0s-MmemZj0iv06QLJpiNhpOEHccYiJTgeAskNOWtXxIFdhoCrUYQAvD_BwE" xr:uid="{0FB896CA-FEB2-49BE-B56E-71A9F627FA4E}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{14FF0BA6-C637-4C91-B94F-D9D5AC390328}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{AA090009-CE3F-4B35-82FF-326E27EDA40A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Schaltplan and Stückliste
</commit_message>
<xml_diff>
--- a/Stuecklisten/Elektrobox_Stückliste.xlsx
+++ b/Stuecklisten/Elektrobox_Stückliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HTL\SPL\CandyMaschine_Project\CandyMachine_Watermelon\Stuecklisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB4C4F6-D5ED-4562-8343-F1392741895F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5946F1D0-1E1E-47C8-BFCF-1F30AA65D87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9960" xr2:uid="{9DA56051-2903-42FB-B064-034924F5A5D2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Anzahl</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Spannungsverteiler</t>
   </si>
   <si>
-    <t>Spannungswandler</t>
-  </si>
-  <si>
     <t>H-Brücke</t>
   </si>
   <si>
@@ -72,12 +69,6 @@
   </si>
   <si>
     <t>B0DG8Z24NN</t>
-  </si>
-  <si>
-    <t>https://www.amazon.de/Spannungs-wandler-Aideepen-Spannungs-regler-Convertermit-Kabelschnittstelle/dp/B0CLRSFL13/ref=sr_1_6?dib=eyJ2IjoiMSJ9.iNDu1-G-hZSMpfKt3KWQqsizmOTcYsYdeO2m0vULZM_UYmGP2L0Uu20hEGeYqkcLr4cjI8LYJIXPR8kVq0czpqGZIl0VCpBIpxlGvgm-q4w_TyiOcCevbTvSzmemBj0379m8slUqp9kocFUlyzWhWErd8Ur4JCNzqblAo8_Xk6NSWKrziujtADu9lubJ_Oud6ZNk17QPVhdYKVY_XBjkGo2EGX_CN0wL8Mc7AvgPTvyDyksc9hjqLexgsVDCZBo3T3LF3aNnpds4ziIuFFaA5ZlESrvCntYASwP1AIsQCak.R0lnyivqmDQa180s2ByuqBlWvAulUb9ms-w3STDRGtk&amp;dib_tag=se&amp;keywords=spannungswandler%2B12v%2B5v&amp;qid=1768547011&amp;sr=8-6&amp;th=1</t>
-  </si>
-  <si>
-    <t>‎A7040220</t>
   </si>
   <si>
     <t>https://www.conrad.at/de/p/tru-components-yst-1102a-drucktaster-12-v-dc-0-05-a-1-x-aus-ein-tastend-l-x-b-6-mm-x-6-mm-1-st-1569018.html?insert=UP&amp;utm_source=google-shopping-de&amp;utm_medium=search&amp;utm_campaign=shopping-online-de&amp;utm_content=shopping-ad_cpc&amp;WT.srch=1&amp;ef_id=CjwKCAiAvaLLBhBFEiwAYCNTf908VSnv0s-MmemZj0iv06QLJpiNhpOEHccYiJTgeAskNOWtXxIFdhoCrUYQAvD_BwE:G:s&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_AT_2025&amp;utm_id=22317741252&amp;gad_source=1&amp;gad_campaignid=22317741252&amp;gclid=CjwKCAiAvaLLBhBFEiwAYCNTf908VSnv0s-MmemZj0iv06QLJpiNhpOEHccYiJTgeAskNOWtXxIFdhoCrUYQAvD_BwE</t>
@@ -270,13 +261,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>808080</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>26400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>831120</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>139080</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -679,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C109D0D-11F1-44AC-92C4-98F0FB4A2F8E}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,13 +706,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" s="4">
         <v>19.8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E2" s="10">
         <v>7630049203969</v>
@@ -729,10 +720,10 @@
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="6">
         <v>5.29</v>
@@ -741,87 +732,69 @@
         <v>5</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C4" s="6">
-        <v>8.0500000000000007</v>
+        <v>24.19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="6">
-        <v>24.19</v>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5">
+        <v>8.56</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="5">
-        <v>8.56</v>
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="9">
+      <c r="E6" s="9">
         <v>2050005748030</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="https://www.amazon.de/Spannungs-wandler-Aideepen-Spannungs-regler-Convertermit-Kabelschnittstelle/dp/B0CLRSFL13/ref=sr_1_6?dib=eyJ2IjoiMSJ9.iNDu1-G-hZSMpfKt3KWQqsizmOTcYsYdeO2m0vULZM_UYmGP2L0Uu20hEGeYqkcLr4cjI8LYJIXPR8kVq0czpqGZIl0VCpBIpxlGvgm-q4w_TyiOcCevbTvSzmemBj0379m8slUqp9kocFUlyzWhWErd8Ur4JCNzqblAo8_Xk6NSWKrziujtADu9lubJ_Oud6ZNk17QPVhdYKVY_XBjkGo2EGX_CN0wL8Mc7AvgPTvyDyksc9hjqLexgsVDCZBo3T3LF3aNnpds4ziIuFFaA5ZlESrvCntYASwP1AIsQCak.R0lnyivqmDQa180s2ByuqBlWvAulUb9ms-w3STDRGtk&amp;dib_tag=se&amp;keywords=spannungswandler%2B12v%2B5v&amp;qid=1768547011&amp;sr=8-6&amp;th=1" xr:uid="{23BD11BB-0F37-4191-8468-10AC86A9F4FE}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00BC4F0C-D697-4CE4-8278-4A347B796AA4}"/>
-    <hyperlink ref="B7" r:id="rId3" display="https://www.conrad.at/de/p/tru-components-yst-1102a-drucktaster-12-v-dc-0-05-a-1-x-aus-ein-tastend-l-x-b-6-mm-x-6-mm-1-st-1569018.html?insert=UP&amp;utm_source=google-shopping-de&amp;utm_medium=search&amp;utm_campaign=shopping-online-de&amp;utm_content=shopping-ad_cpc&amp;WT.srch=1&amp;ef_id=CjwKCAiAvaLLBhBFEiwAYCNTf908VSnv0s-MmemZj0iv06QLJpiNhpOEHccYiJTgeAskNOWtXxIFdhoCrUYQAvD_BwE:G:s&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_AT_2025&amp;utm_id=22317741252&amp;gad_source=1&amp;gad_campaignid=22317741252&amp;gclid=CjwKCAiAvaLLBhBFEiwAYCNTf908VSnv0s-MmemZj0iv06QLJpiNhpOEHccYiJTgeAskNOWtXxIFdhoCrUYQAvD_BwE" xr:uid="{0FB896CA-FEB2-49BE-B56E-71A9F627FA4E}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{14FF0BA6-C637-4C91-B94F-D9D5AC390328}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{AA090009-CE3F-4B35-82FF-326E27EDA40A}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00BC4F0C-D697-4CE4-8278-4A347B796AA4}"/>
+    <hyperlink ref="B6" r:id="rId2" display="https://www.conrad.at/de/p/tru-components-yst-1102a-drucktaster-12-v-dc-0-05-a-1-x-aus-ein-tastend-l-x-b-6-mm-x-6-mm-1-st-1569018.html?insert=UP&amp;utm_source=google-shopping-de&amp;utm_medium=search&amp;utm_campaign=shopping-online-de&amp;utm_content=shopping-ad_cpc&amp;WT.srch=1&amp;ef_id=CjwKCAiAvaLLBhBFEiwAYCNTf908VSnv0s-MmemZj0iv06QLJpiNhpOEHccYiJTgeAskNOWtXxIFdhoCrUYQAvD_BwE:G:s&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_AT_2025&amp;utm_id=22317741252&amp;gad_source=1&amp;gad_campaignid=22317741252&amp;gclid=CjwKCAiAvaLLBhBFEiwAYCNTf908VSnv0s-MmemZj0iv06QLJpiNhpOEHccYiJTgeAskNOWtXxIFdhoCrUYQAvD_BwE" xr:uid="{0FB896CA-FEB2-49BE-B56E-71A9F627FA4E}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{14FF0BA6-C637-4C91-B94F-D9D5AC390328}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{AA090009-CE3F-4B35-82FF-326E27EDA40A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId6"/>
-  <drawing r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>